<commit_message>
bulk upload properties sample changes
</commit_message>
<xml_diff>
--- a/zoyAdminAngular/src/assets/sample_files/PG_properties_sample_file.xlsx
+++ b/zoyAdminAngular/src/assets/sample_files/PG_properties_sample_file.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28521"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bulk-upload-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_8336292F024F7602ADCBAE6509902CF5B9A85CDF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EEEF1AB-E15C-4C82-9DAD-36FFD3793362}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Floor Name</t>
   </si>
@@ -52,7 +53,7 @@
     <t>Room Area in Sqft</t>
   </si>
   <si>
-    <t>Daily Rent</t>
+    <t>Available Bed Numbers</t>
   </si>
   <si>
     <t>Monthly Rent</t>
@@ -61,9 +62,6 @@
     <t>Room Amenities</t>
   </si>
   <si>
-    <t>Occupied Bed Numbers</t>
-  </si>
-  <si>
     <t>Remarks About Room</t>
   </si>
   <si>
@@ -85,9 +83,6 @@
     <t>Mandatory</t>
   </si>
   <si>
-    <t xml:space="preserve">Mandatory for Occupaid Beds </t>
-  </si>
-  <si>
     <t>Optional - 300 Cherecters</t>
   </si>
   <si>
@@ -109,9 +104,6 @@
     <t>Air-conditioning,Food-Breakfast,Food-Lunch,Food-Dinner,TV,Parking,Wi-Fi</t>
   </si>
   <si>
-    <t>101-A</t>
-  </si>
-  <si>
     <t>Spacious room</t>
   </si>
   <si>
@@ -148,9 +140,6 @@
     <t>201-B,201-C,201-D</t>
   </si>
   <si>
-    <t>201-A</t>
-  </si>
-  <si>
     <t>Room 202</t>
   </si>
   <si>
@@ -161,16 +150,13 @@
   </si>
   <si>
     <t>203-A</t>
-  </si>
-  <si>
-    <t>Available Bed Numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,30 +513,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="69.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -567,259 +551,219 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="6">
         <v>1000</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6">
+        <v>8000</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6">
-        <v>500</v>
-      </c>
-      <c r="H3" s="6">
-        <v>8000</v>
-      </c>
-      <c r="I3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="E4" s="6">
         <v>850</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6">
+        <v>8000</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="G4" s="6">
-        <v>500</v>
-      </c>
-      <c r="H4" s="6">
-        <v>8000</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="6">
         <v>500</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G5" s="6">
-        <v>500</v>
-      </c>
-      <c r="H5" s="6">
         <v>8000</v>
       </c>
+      <c r="H5" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6">
         <v>1000</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G6" s="6">
-        <v>500</v>
-      </c>
-      <c r="H6" s="6">
         <v>8000</v>
       </c>
+      <c r="H6" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="I6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="E7" s="6">
         <v>850</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G7" s="6">
-        <v>500</v>
-      </c>
-      <c r="H7" s="6">
         <v>8000</v>
       </c>
+      <c r="H7" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="I7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E8" s="6">
         <v>500</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G8" s="6">
-        <v>500</v>
-      </c>
-      <c r="H8" s="6">
         <v>8000</v>
       </c>
+      <c r="H8" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>